<commit_message>
update excel dan buat 2 model
</commit_message>
<xml_diff>
--- a/Test excel/PemenuhanMutu.xlsx
+++ b/Test excel/PemenuhanMutu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LPMPS\Test excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52449D2-92AE-4189-89E1-6CA9992EA824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96C61FD-7946-406A-8DA4-A5266BAAF323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E604F1CB-8D65-4249-BE23-B6E2CB777384}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E604F1CB-8D65-4249-BE23-B6E2CB777384}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="128">
   <si>
     <t>No</t>
   </si>
@@ -148,6 +148,267 @@
   </si>
   <si>
     <t>6.03</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sekolah melaksanakan kurikulum sesuai ketentuan </t>
+  </si>
+  <si>
+    <t>1.3.1</t>
+  </si>
+  <si>
+    <t>1.3.2</t>
+  </si>
+  <si>
+    <t>1.3.3</t>
+  </si>
+  <si>
+    <t>1.3.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menyediakan alokasi waktu pembelajaran sesuai struktur kurikulum yang berlaku </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mengatur beban belajar berdasarkan bentuk pendalaman materi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menyelenggarakan aspek kurikulum pada muatan local </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melaksanakan kegiatan pengembangan diri siswa </t>
+  </si>
+  <si>
+    <t>2.85</t>
+  </si>
+  <si>
+    <t>6.53</t>
+  </si>
+  <si>
+    <t>6.54</t>
+  </si>
+  <si>
+    <t>Proses</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sekolah merencanakan proses pembelajaran sesuai ketentuan </t>
+  </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>2.1.2</t>
+  </si>
+  <si>
+    <t>2.1.3</t>
+  </si>
+  <si>
+    <t>2.1.4</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mengacu pada silabus yang telah dikembangkan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mengarah pada pencapaian kompetensi </t>
+  </si>
+  <si>
+    <t>6.76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menyusun dokumen rencana dengan lengkap dan sistematis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mendapatkan evaluasi dari kepala sekolah dan pengawas sekolah </t>
+  </si>
+  <si>
+    <t>6.48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proses pembelajaran dilaksanakan dengan tepat </t>
+  </si>
+  <si>
+    <t>2.2.1</t>
+  </si>
+  <si>
+    <t>2.2.2</t>
+  </si>
+  <si>
+    <t>2.2.3</t>
+  </si>
+  <si>
+    <t>2.2.4</t>
+  </si>
+  <si>
+    <t>2.2.5</t>
+  </si>
+  <si>
+    <t>2.2.6</t>
+  </si>
+  <si>
+    <t>2.2.7</t>
+  </si>
+  <si>
+    <t>2.2.8</t>
+  </si>
+  <si>
+    <t>2.2.9</t>
+  </si>
+  <si>
+    <t>2.2.10</t>
+  </si>
+  <si>
+    <t>2.2.11</t>
+  </si>
+  <si>
+    <t>2.2.12</t>
+  </si>
+  <si>
+    <t>2.2.13</t>
+  </si>
+  <si>
+    <t>2.2.14</t>
+  </si>
+  <si>
+    <t>2.2.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Membentuk rombongan belajar dengan jumlah siswa sesuai ketentuan </t>
+  </si>
+  <si>
+    <t>6.88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mengelola kelas sebelum memulai pembelajaran </t>
+  </si>
+  <si>
+    <t>4.69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mendorong siswa mencari tahu </t>
+  </si>
+  <si>
+    <t>Mengarahkan pada penggunaan pendekatan ilmiah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melakukan pembelajaran berbasis kompetensi </t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memberikan pembelajaran terpadu </t>
+  </si>
+  <si>
+    <t>Melaksanakan pembelajaran dengan jawaban yang kebenarannya multi dimensi</t>
+  </si>
+  <si>
+    <t>6.41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melaksanakan pembelajaran menuju pada keterampilan aplikatif </t>
+  </si>
+  <si>
+    <t>6.37</t>
+  </si>
+  <si>
+    <t>Mengutamakan  pemberdayaan siswa sebagai pembelajar sepanjang hayat</t>
+  </si>
+  <si>
+    <t>6.9</t>
+  </si>
+  <si>
+    <t>Menerapkan prinsip bahwa siapa saja adalah guru, siapa saja adalah siswa, dan di mana saja adalah kelas.</t>
+  </si>
+  <si>
+    <t>6.72</t>
+  </si>
+  <si>
+    <t>Mengakui atas perbedaan individual dan latar belakang budaya siswa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menerapkan metode pembelajaran sesuai karakteristik siswa </t>
+  </si>
+  <si>
+    <t>4.57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memanfaatkan media pembelajaran dalam meningkatkan efisiensi dan efektivitas pembelajaran </t>
+  </si>
+  <si>
+    <t>5.93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menggunakan aneka sumber belajar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mengelola kelas saat menutup pembelajaran  </t>
+  </si>
+  <si>
+    <t>6.66</t>
+  </si>
+  <si>
+    <t>2.3.1</t>
+  </si>
+  <si>
+    <t>2.3.2</t>
+  </si>
+  <si>
+    <t>2.3.3</t>
+  </si>
+  <si>
+    <t>2.3.4</t>
+  </si>
+  <si>
+    <t>2.3.5</t>
+  </si>
+  <si>
+    <t>2.3.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melakukan penilaian otentik secara komprehensif </t>
+  </si>
+  <si>
+    <t>3.57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memanfaatkan hasil penilaian otentik </t>
+  </si>
+  <si>
+    <t>4.66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melakukan pemantauan proses pembelajaran </t>
+  </si>
+  <si>
+    <t>5.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melakukan supervisi proses pembelajaran kepada guru </t>
+  </si>
+  <si>
+    <t>5.29</t>
+  </si>
+  <si>
+    <t>Mengevaluasi proses pembelajaran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menindaklanjuti hasil pengawasan proses pembelajaran </t>
+  </si>
+  <si>
+    <t>5.97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pengawasan dan penilaian otentik dilakukan dalam proses pembelajaran </t>
   </si>
 </sst>
 </file>
@@ -225,40 +486,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,212 +845,212 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8062AF8-CD22-4F37-85A0-2378D2A76DCE}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" customWidth="1"/>
+    <col min="7" max="7" width="17.6328125" customWidth="1"/>
+    <col min="8" max="8" width="15.36328125" customWidth="1"/>
+    <col min="10" max="10" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>31</v>
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+    <row r="2" spans="1:10" ht="56.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
-        <v>2021</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4">
-        <v>2021</v>
-      </c>
-      <c r="C3" s="4">
+    <row r="3" spans="1:10" ht="56.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+    <row r="4" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
-        <v>2021</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="B4" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+    <row r="5" spans="1:10" ht="56.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
-        <v>2021</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="B5" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+    <row r="6" spans="1:10" ht="56.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
-        <v>2021</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="B6" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+    <row r="7" spans="1:10" ht="65.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
-        <v>2021</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="B7" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -791,24 +1062,24 @@
       <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+    <row r="8" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
-        <v>2021</v>
-      </c>
-      <c r="C8" s="4">
+      <c r="B8" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C8" s="2">
         <v>1</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="8" t="s">
@@ -820,24 +1091,24 @@
       <c r="H8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+    <row r="9" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
-        <v>2021</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="B9" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C9" s="2">
         <v>1</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="8" t="s">
@@ -849,24 +1120,24 @@
       <c r="H9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+    <row r="10" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
-        <v>2021</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C10" s="2">
         <v>1</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="8" t="s">
@@ -878,8 +1149,849 @@
       <c r="H10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="7" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="78.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="39.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="39.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="I15" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="39.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="65.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="39.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="39.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="39.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="39.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="65.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="65.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="65.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="3">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C27" s="3">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="78.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C28" s="3">
+        <v>2</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="65.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C29" s="3">
+        <v>2</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C30" s="3">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="91.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="39.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="39.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="3">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C33" s="3">
+        <v>2</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C34" s="3">
+        <v>2</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="3">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C35" s="3">
+        <v>2</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="3">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C36" s="3">
+        <v>2</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="3">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="3">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C38" s="3">
+        <v>2</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="3">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C39" s="3">
+        <v>2</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>